<commit_message>
heel veel dingen veranderd
</commit_message>
<xml_diff>
--- a/Documentatie/tijdsplanning.xlsx
+++ b/Documentatie/tijdsplanning.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="9324"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="9324" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blad1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>Wie</t>
   </si>
@@ -108,6 +109,15 @@
   </si>
   <si>
     <t>personeel realisatie</t>
+  </si>
+  <si>
+    <t>mockup links</t>
+  </si>
+  <si>
+    <t>wireframe links</t>
+  </si>
+  <si>
+    <t>Links realisatie</t>
   </si>
 </sst>
 </file>
@@ -139,7 +149,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -173,6 +183,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -190,124 +211,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -583,10 +507,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,8 +540,8 @@
         <v>3</v>
       </c>
       <c r="B1" s="3">
-        <f>SUM(D4:D19)</f>
-        <v>18.25</v>
+        <f>SUM(D4:D21)</f>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -646,7 +582,7 @@
       <c r="E4" s="8">
         <v>42867</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="2"/>
@@ -665,7 +601,7 @@
       <c r="E5" s="8">
         <v>42867</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -683,7 +619,9 @@
       <c r="E6" s="8">
         <v>42874</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -700,7 +638,9 @@
       <c r="E7" s="8">
         <v>42874</v>
       </c>
-      <c r="F7" s="11"/>
+      <c r="F7" s="10" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
@@ -716,30 +656,40 @@
       <c r="E8" s="8">
         <v>42874</v>
       </c>
-      <c r="F8" s="11"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="13">
+        <v>0.75</v>
+      </c>
+      <c r="E9" s="5">
+        <v>42874</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-      <c r="E10" s="8">
-        <v>42874</v>
-      </c>
-      <c r="F10" s="11"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6">
@@ -748,14 +698,14 @@
       <c r="E11" s="8">
         <v>42874</v>
       </c>
-      <c r="F11" s="11"/>
+      <c r="F11" s="10"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6">
@@ -764,14 +714,14 @@
       <c r="E12" s="8">
         <v>42874</v>
       </c>
-      <c r="F12" s="11"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6">
@@ -780,14 +730,14 @@
       <c r="E13" s="8">
         <v>42874</v>
       </c>
-      <c r="F13" s="11"/>
+      <c r="F13" s="10"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6">
@@ -796,113 +746,121 @@
       <c r="E14" s="8">
         <v>42874</v>
       </c>
-      <c r="F14" s="11"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6">
+        <v>1</v>
+      </c>
+      <c r="E15" s="8">
+        <v>42874</v>
+      </c>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="13">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>42874</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6">
         <v>1.5</v>
       </c>
-      <c r="E16" s="8">
-        <v>42874</v>
-      </c>
-      <c r="F16" s="11"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="E17" s="8">
-        <v>42874</v>
-      </c>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="E18" s="4">
-        <v>42881</v>
-      </c>
-      <c r="F18" s="6"/>
+      <c r="E18" s="8">
+        <v>42874</v>
+      </c>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15">
-        <v>2</v>
-      </c>
-      <c r="E19" s="4">
-        <v>42881</v>
-      </c>
-      <c r="F19" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="E19" s="8">
+        <v>42874</v>
+      </c>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="15">
-        <v>2</v>
+      <c r="D20" s="5">
+        <v>2.5</v>
       </c>
       <c r="E20" s="4">
         <v>42881</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="14">
+        <v>21</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13">
         <v>2</v>
       </c>
       <c r="E21" s="4">
         <v>42881</v>
       </c>
-      <c r="F21" s="5"/>
+      <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>23</v>
+      <c r="B22" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="14">
+      <c r="D22" s="13">
         <v>2</v>
       </c>
       <c r="E22" s="4">
@@ -911,192 +869,58 @@
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="5"/>
+      <c r="D23" s="12">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4">
+        <v>42881</v>
+      </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
+      <c r="A24" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="5"/>
+      <c r="D24" s="12">
+        <v>2</v>
+      </c>
+      <c r="E24" s="4">
+        <v>42881</v>
+      </c>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
+      <c r="A25" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
+      <c r="D25" s="5">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4">
+        <v>42881</v>
+      </c>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="10"/>
-      <c r="B44" s="10"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="13"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B23:E43">
-    <cfRule type="expression" dxfId="7" priority="4">
-      <formula>$E23 &gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23:A43">
-    <cfRule type="expression" dxfId="6" priority="33">
-      <formula>$E23 &gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
+  <mergeCells count="2">
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A17:F17"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
mockups in psd en png vorm + kleine aanpassing tijdsplanning
</commit_message>
<xml_diff>
--- a/Documentatie/tijdsplanning.xlsx
+++ b/Documentatie/tijdsplanning.xlsx
@@ -522,7 +522,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,7 +669,7 @@
       <c r="D9" s="13">
         <v>0.75</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>42874</v>
       </c>
       <c r="F9" s="15" t="s">
@@ -760,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="8">
-        <v>42874</v>
+        <v>42881</v>
       </c>
       <c r="F15" s="10"/>
     </row>
@@ -776,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="4">
-        <v>42874</v>
+        <v>42881</v>
       </c>
       <c r="F16" s="5"/>
     </row>
@@ -800,7 +800,7 @@
         <v>1.5</v>
       </c>
       <c r="E18" s="8">
-        <v>42874</v>
+        <v>42881</v>
       </c>
       <c r="F18" s="10"/>
     </row>
@@ -816,7 +816,7 @@
         <v>1.5</v>
       </c>
       <c r="E19" s="8">
-        <v>42874</v>
+        <v>42881</v>
       </c>
       <c r="F19" s="11"/>
     </row>
@@ -848,7 +848,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="4">
-        <v>42881</v>
+        <v>42888</v>
       </c>
       <c r="F21" s="6"/>
     </row>
@@ -864,7 +864,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="4">
-        <v>42881</v>
+        <v>42888</v>
       </c>
       <c r="F22" s="5"/>
     </row>
@@ -880,7 +880,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="4">
-        <v>42881</v>
+        <v>42888</v>
       </c>
       <c r="F23" s="5"/>
     </row>
@@ -896,7 +896,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="4">
-        <v>42881</v>
+        <v>42888</v>
       </c>
       <c r="F24" s="5"/>
     </row>
@@ -912,7 +912,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="4">
-        <v>42881</v>
+        <v>42888</v>
       </c>
       <c r="F25" s="5"/>
     </row>

</xml_diff>

<commit_message>
tijdsplanning excel bestand en logo.jpg
</commit_message>
<xml_diff>
--- a/Documentatie/tijdsplanning.xlsx
+++ b/Documentatie/tijdsplanning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>Wie</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>header</t>
-  </si>
-  <si>
-    <t>footer</t>
   </si>
   <si>
     <t>Stan</t>
@@ -214,17 +211,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -519,10 +516,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,8 +537,8 @@
         <v>3</v>
       </c>
       <c r="B1" s="3">
-        <f>SUM(D4:D21)</f>
-        <v>20</v>
+        <f>SUM(D4:D20)</f>
+        <v>18.5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -556,24 +553,24 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6">
@@ -583,16 +580,16 @@
         <v>42867</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6">
@@ -602,15 +599,15 @@
         <v>42867</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6">
@@ -620,16 +617,16 @@
         <v>42874</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6">
@@ -639,15 +636,15 @@
         <v>42874</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6">
@@ -656,24 +653,26 @@
       <c r="E8" s="8">
         <v>42874</v>
       </c>
-      <c r="F8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <v>0.75</v>
       </c>
       <c r="E9" s="4">
         <v>42874</v>
       </c>
-      <c r="F9" s="15" t="s">
-        <v>25</v>
+      <c r="F9" s="13" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -686,10 +685,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6">
@@ -698,14 +697,16 @@
       <c r="E11" s="8">
         <v>42874</v>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6">
@@ -714,14 +715,16 @@
       <c r="E12" s="8">
         <v>42874</v>
       </c>
-      <c r="F12" s="10"/>
+      <c r="F12" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6">
@@ -730,14 +733,16 @@
       <c r="E13" s="8">
         <v>42874</v>
       </c>
-      <c r="F13" s="10"/>
+      <c r="F13" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6">
@@ -746,14 +751,16 @@
       <c r="E14" s="8">
         <v>42874</v>
       </c>
-      <c r="F14" s="10"/>
+      <c r="F14" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6">
@@ -762,23 +769,27 @@
       <c r="E15" s="8">
         <v>42881</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="10" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="13">
+      <c r="D16" s="12">
         <v>1</v>
       </c>
       <c r="E16" s="4">
         <v>42881</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="15" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
@@ -789,11 +800,11 @@
       <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>8</v>
+      <c r="A18" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6">
@@ -805,116 +816,100 @@
       <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="E19" s="8">
+      <c r="A19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="E19" s="4">
         <v>42881</v>
       </c>
-      <c r="F19" s="11"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5">
-        <v>2.5</v>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12">
+        <v>2</v>
       </c>
       <c r="E20" s="4">
-        <v>42881</v>
-      </c>
-      <c r="F20" s="6"/>
+        <v>42888</v>
+      </c>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13">
+        <v>26</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="12">
         <v>2</v>
       </c>
       <c r="E21" s="4">
         <v>42888</v>
       </c>
-      <c r="F21" s="6"/>
+      <c r="F21" s="15"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="13">
+      <c r="D22" s="11">
         <v>2</v>
       </c>
       <c r="E22" s="4">
         <v>42888</v>
       </c>
-      <c r="F22" s="5"/>
+      <c r="F22" s="15"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="12">
+      <c r="D23" s="11">
         <v>2</v>
       </c>
       <c r="E23" s="4">
         <v>42888</v>
       </c>
-      <c r="F23" s="5"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>23</v>
+      <c r="B24" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="12">
+      <c r="D24" s="5">
         <v>2</v>
       </c>
       <c r="E24" s="4">
         <v>42888</v>
       </c>
-      <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5">
-        <v>2</v>
-      </c>
-      <c r="E25" s="4">
-        <v>42888</v>
-      </c>
-      <c r="F25" s="5"/>
+      <c r="F24" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>